<commit_message>
Started routing the PCB, adding cut-outs to separate the analog from digital signal-domains.
</commit_message>
<xml_diff>
--- a/Docs/Changelog.xlsx
+++ b/Docs/Changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Teknikprojekt\Hardware\MSX\trh9000\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAD0E0A-1676-42AC-AD0E-9A8D0E2871F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24676F67-128E-4BB5-A457-6AC31BC70665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>Removed Composite video and replaced with RGB Scart</t>
+  </si>
+  <si>
+    <t>Made a 3D-model for the LQFP-128 package (V9990)</t>
+  </si>
+  <si>
+    <t>Replaced some decoupling capacitors for bigger ones.</t>
+  </si>
+  <si>
+    <t>Changed 21MHz crystal to SMD.</t>
+  </si>
+  <si>
+    <t>Corrected and error with labeling two parts of a symbol different numbers.</t>
+  </si>
+  <si>
+    <t>Started routing the PCB, adding cut-outs to separate the analog from digital signal-domains.</t>
   </si>
 </sst>
 </file>
@@ -498,7 +513,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,24 +595,40 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="2">
+        <v>44788</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="2">
+        <v>44789</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="2">
+        <v>44793</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>

</xml_diff>

<commit_message>
More adjustments of layout.
</commit_message>
<xml_diff>
--- a/Docs/Changelog.xlsx
+++ b/Docs/Changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Teknikprojekt\Hardware\MSX\trh9000\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24676F67-128E-4BB5-A457-6AC31BC70665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F30574-AC12-47B8-89AC-6861294E8026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -513,13 +513,13 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -575,6 +575,9 @@
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -601,6 +604,9 @@
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -608,6 +614,9 @@
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,6 +637,9 @@
       </c>
       <c r="B14" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More routing of the analog portion. Added 3D-models for the VGA and Scart connectors.
</commit_message>
<xml_diff>
--- a/Docs/Changelog.xlsx
+++ b/Docs/Changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Teknikprojekt\Hardware\MSX\trh9000\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F30574-AC12-47B8-89AC-6861294E8026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D78C3B-664E-4177-9411-E123521D0318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Started routing the PCB, adding cut-outs to separate the analog from digital signal-domains.</t>
+  </si>
+  <si>
+    <t>Added PTC-fuse and power-on indication-LED.</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,8 +646,12 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="2">
+        <v>44796</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>

</xml_diff>